<commit_message>
updated notebook and requirements
</commit_message>
<xml_diff>
--- a/smiles_curated.xlsx
+++ b/smiles_curated.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,86 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -494,7 +562,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>O=[N+]([O-])c1cccc(P(=O)(O)O)c1</t>
+          <t>O=[N+]([O-])c1cc(P(=O)(O)O)ccc1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -591,7 +659,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>inorganic_salt</t>
+          <t>no_sanitizable</t>
         </is>
       </c>
     </row>
@@ -609,7 +677,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Clc1cc2c(oc3cc(Cl)c(Cl)c(Cl)c32)c(Cl)c1Cl</t>
+          <t>Clc1c(Cl)c(Cl)c2oc3c(c(Cl)c(Cl)c(Cl)c3)c2c1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -655,7 +723,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Nc1ccc2c([O-])c(N=Nc3ccc(-c4ccc(N=Nc5c(S(=O)(=O)O)cc6cc(N)ccc6c5[O-])cc4)cc3)c(S(=O)(=O)O)cc2c1.[Na+].[Na+]</t>
+          <t>Nc1cc2cc(S(=O)(=O)O)c(N=Nc3ccc(-c4ccc(N=Nc5c(S(=O)(=O)O)cc6cc(N)ccc6c5[O-])cc4)cc3)c([O-])c2cc1.[Na+].[Na+]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -849,6 +917,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
salt remover properly working
</commit_message>
<xml_diff>
--- a/smiles_curated.xlsx
+++ b/smiles_curated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -446,10 +446,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>meta1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>meta2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>meta3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>structure_curated</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>substance_type_name</t>
         </is>
@@ -469,10 +484,25 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Cc1ccc(Cl)cc1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -492,10 +522,25 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>N#CN</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -515,10 +560,25 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Oc1ccc(Cl)c(Cl)c1</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -538,10 +598,25 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>CC(c1ccccc1)c1ccc(OCCOCCO)cc1</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -561,10 +636,25 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>O=[N+]([O-])c1cc(P(=O)(O)O)ccc1</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -584,10 +674,25 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>CCCCCCCCCCOCCO</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -607,10 +712,25 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>CN(C)CCO</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -630,10 +750,25 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[Cl-].[K+]</t>
+          <t>dummy</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>[K+]</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>inorganic_salt</t>
         </is>
@@ -653,10 +788,25 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>[Cu+].[Cu+].[OH2-2]</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>no_sanitizable</t>
         </is>
@@ -676,10 +826,25 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Clc1c(Cl)c(Cl)c2oc3c(c(Cl)c(Cl)c(Cl)c3)c2c1</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -699,10 +864,25 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Cc1cc(-c2ccc(N)c(C)c2)ccc1N</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -722,10 +902,25 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Nc1cc2cc(S(=O)(=O)O)c(N=Nc3ccc(-c4ccc(N=Nc5c(S(=O)(=O)O)cc6cc(N)ccc6c5[O-])cc4)cc3)c([O-])c2cc1.[Na+].[Na+]</t>
+          <t>dummy</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nc1ccc2c([O-])c(N=Nc3ccc(-c4ccc(N=Nc5c(S(=O)(=O)O)cc6cc(N)ccc6c5[O-])cc4)cc3)c(S(=O)(=O)O)cc2c1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>organic_salt</t>
         </is>
@@ -745,10 +940,25 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>Clc1cc2c(cc1Cl)Oc1c(Cl)c(Cl)c(Cl)c(Cl)c1O2</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -768,10 +978,25 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Cc1ccccc1N=Nc1c(N)ccc2ccccc12</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -791,10 +1016,25 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>CCCCOCCOC(C)=O</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -814,10 +1054,25 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>C=CC(=O)NCO</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -837,10 +1092,25 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>O.O=S(=O)([O-])[O-].[Zn+2]</t>
+          <t>dummy</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>O=S(=O)([O-])[O-]</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>inorganic_salt</t>
         </is>
@@ -860,10 +1130,25 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[O-2].[O-2].[O-2].[Sb+3].[Sb+3]</t>
+          <t>dummy</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>[Sb+3]</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>inorganic_salt</t>
         </is>
@@ -883,10 +1168,25 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>COc1ccc(/C=C/C(=O)Nc2ccc(C(N)=O)cc2)cc1</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>organic</t>
         </is>
@@ -906,10 +1206,25 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>dummy</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>CO</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>organic</t>
         </is>

</xml_diff>